<commit_message>
use cases: marrage before divorce and marrage before death complets. gedcom file edits.
</commit_message>
<xml_diff>
--- a/Project Sprint Report.xlsx
+++ b/Project Sprint Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="400" windowWidth="26780" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2115" yWindow="405" windowWidth="26775" windowHeight="15540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId7"/>
     <sheet name="Stories" sheetId="11" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="185">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -605,6 +605,12 @@
   </si>
   <si>
     <t>https://github.com/kichithewolf/CS-555-Project</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -820,6 +826,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -853,10 +864,10 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41169.0</c:v>
+                  <c:v>41169</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41173.0</c:v>
+                  <c:v>41173</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -868,10 +879,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -888,11 +899,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2091466360"/>
-        <c:axId val="2091469448"/>
+        <c:axId val="179481600"/>
+        <c:axId val="180294400"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2091466360"/>
+        <c:axId val="179481600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -902,14 +913,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091469448"/>
+        <c:crossAx val="180294400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2091469448"/>
+        <c:axId val="180294400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,7 +931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091466360"/>
+        <c:crossAx val="179481600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -931,7 +942,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1298,15 +1309,15 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="6.375" customWidth="1"/>
+    <col min="2" max="2" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -1323,7 +1334,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -1340,7 +1351,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>170</v>
       </c>
@@ -1357,7 +1368,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>171</v>
       </c>
@@ -1374,7 +1385,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -1408,20 +1419,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D7"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="7.75" customWidth="1"/>
+    <col min="3" max="3" width="23.375" customWidth="1"/>
+    <col min="4" max="4" width="6.75" customWidth="1"/>
+    <col min="5" max="5" width="7.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -1438,7 +1449,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1452,7 +1463,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1466,7 +1477,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1479,8 +1490,11 @@
       <c r="D4" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1493,8 +1507,11 @@
       <c r="D5" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1508,7 +1525,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1539,20 +1556,20 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="2"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.75" style="2"/>
+    <col min="2" max="2" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1572,7 +1589,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>41169</v>
       </c>
@@ -1583,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>41173</v>
       </c>
@@ -1622,23 +1639,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="6"/>
+    <col min="1" max="1" width="7.75" customWidth="1"/>
+    <col min="2" max="2" width="24.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.75" customWidth="1"/>
+    <col min="5" max="5" width="9.75" customWidth="1"/>
+    <col min="6" max="6" width="10.75" customWidth="1"/>
+    <col min="7" max="7" width="9.25" customWidth="1"/>
+    <col min="8" max="8" width="12.125" customWidth="1"/>
+    <col min="9" max="9" width="10.75" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -1667,7 +1684,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -1684,7 +1701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -1701,7 +1718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -1711,14 +1728,26 @@
       <c r="C4" t="s">
         <v>171</v>
       </c>
+      <c r="D4" t="s">
+        <v>183</v>
+      </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -1728,14 +1757,26 @@
       <c r="C5" t="s">
         <v>171</v>
       </c>
+      <c r="D5" t="s">
+        <v>183</v>
+      </c>
       <c r="E5">
         <v>5</v>
       </c>
       <c r="F5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -1752,7 +1793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -1769,36 +1810,36 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="26">
+    <row r="21" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1823,9 +1864,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -1874,9 +1915,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -1924,9 +1965,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -1971,16 +2012,16 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.625" customWidth="1"/>
+    <col min="3" max="3" width="49.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>122</v>
       </c>
@@ -1991,7 +2032,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -2002,7 +2043,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -2013,7 +2054,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -2024,7 +2065,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -2035,7 +2076,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15">
+    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -2046,7 +2087,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15">
+    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -2057,7 +2098,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45">
+    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -2068,7 +2109,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -2079,7 +2120,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>131</v>
       </c>
@@ -2090,7 +2131,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -2101,7 +2142,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -2112,7 +2153,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>134</v>
       </c>
@@ -2123,7 +2164,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30">
+    <row r="14" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>135</v>
       </c>
@@ -2134,7 +2175,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15">
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -2145,7 +2186,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -2156,7 +2197,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15">
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -2167,7 +2208,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -2178,7 +2219,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>140</v>
       </c>
@@ -2189,7 +2230,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>141</v>
       </c>
@@ -2200,7 +2241,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15">
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>142</v>
       </c>
@@ -2211,7 +2252,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30">
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>143</v>
       </c>
@@ -2222,7 +2263,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30">
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>144</v>
       </c>
@@ -2233,7 +2274,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>145</v>
       </c>
@@ -2244,7 +2285,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30">
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>146</v>
       </c>
@@ -2255,7 +2296,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30">
+    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>147</v>
       </c>
@@ -2266,7 +2307,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="60">
+    <row r="27" spans="1:3" ht="94.5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>148</v>
       </c>
@@ -2277,7 +2318,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>149</v>
       </c>
@@ -2288,7 +2329,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>150</v>
       </c>
@@ -2299,7 +2340,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>151</v>
       </c>
@@ -2310,7 +2351,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>152</v>
       </c>
@@ -2321,7 +2362,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>153</v>
       </c>
@@ -2332,7 +2373,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>154</v>
       </c>
@@ -2343,7 +2384,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30">
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>155</v>
       </c>
@@ -2354,7 +2395,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30">
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>156</v>
       </c>
@@ -2365,7 +2406,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30">
+    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>157</v>
       </c>
@@ -2376,7 +2417,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15">
+    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>158</v>
       </c>
@@ -2387,7 +2428,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -2398,7 +2439,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30">
+    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>160</v>
       </c>
@@ -2409,7 +2450,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>161</v>
       </c>
@@ -2420,7 +2461,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30">
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>162</v>
       </c>
@@ -2431,7 +2472,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15">
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>163</v>
       </c>
@@ -2442,7 +2483,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>164</v>
       </c>

</xml_diff>

<commit_message>
use cases: list dead and list age complete
</commit_message>
<xml_diff>
--- a/Project Sprint Report.xlsx
+++ b/Project Sprint Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2112" yWindow="408" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="2115" yWindow="405" windowWidth="23250" windowHeight="13170" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId7"/>
     <sheet name="Stories" sheetId="11" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="185">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -905,11 +905,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="94306304"/>
-        <c:axId val="94307840"/>
+        <c:axId val="176397312"/>
+        <c:axId val="176419584"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="94306304"/>
+        <c:axId val="176397312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -919,14 +919,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94307840"/>
+        <c:crossAx val="176419584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="94307840"/>
+        <c:axId val="176419584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,7 +937,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94306304"/>
+        <c:crossAx val="176397312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1315,12 +1315,12 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.36328125" customWidth="1"/>
-    <col min="2" max="2" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" width="6.375" customWidth="1"/>
+    <col min="2" max="2" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1357,7 +1357,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>170</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -1426,16 +1426,16 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.08984375" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" customWidth="1"/>
-    <col min="3" max="3" width="23.36328125" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" customWidth="1"/>
-    <col min="5" max="5" width="7.7265625" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="7.75" customWidth="1"/>
+    <col min="3" max="3" width="23.375" customWidth="1"/>
+    <col min="4" max="4" width="6.75" customWidth="1"/>
+    <col min="5" max="5" width="7.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1598,6 +1598,9 @@
       <c r="D10" t="s">
         <v>171</v>
       </c>
+      <c r="E10" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1639,6 +1642,9 @@
       </c>
       <c r="D13" t="s">
         <v>171</v>
+      </c>
+      <c r="E13" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -1661,14 +1667,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" style="2"/>
-    <col min="2" max="2" width="18.36328125" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" customWidth="1"/>
-    <col min="4" max="4" width="7.08984375" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.6328125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.75" style="2"/>
+    <col min="2" max="2" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1762,20 +1768,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" customWidth="1"/>
-    <col min="2" max="2" width="24.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" customWidth="1"/>
-    <col min="7" max="7" width="9.26953125" customWidth="1"/>
-    <col min="8" max="8" width="12.08984375" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" style="6"/>
+    <col min="1" max="1" width="7.75" customWidth="1"/>
+    <col min="2" max="2" width="24.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.75" customWidth="1"/>
+    <col min="5" max="5" width="9.75" customWidth="1"/>
+    <col min="6" max="6" width="10.75" customWidth="1"/>
+    <col min="7" max="7" width="9.25" customWidth="1"/>
+    <col min="8" max="8" width="12.125" customWidth="1"/>
+    <col min="9" max="9" width="10.75" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -2000,7 +2006,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>37</v>
       </c>
@@ -2010,7 +2016,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>36</v>
       </c>
@@ -2031,13 +2037,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.90625" customWidth="1"/>
+    <col min="2" max="2" width="18.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -2113,11 +2119,23 @@
       <c r="C4" t="s">
         <v>171</v>
       </c>
+      <c r="D4" t="s">
+        <v>183</v>
+      </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4">
         <v>5</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -2164,11 +2182,23 @@
       <c r="C7" t="s">
         <v>171</v>
       </c>
+      <c r="D7" t="s">
+        <v>183</v>
+      </c>
       <c r="E7">
         <v>20</v>
       </c>
       <c r="F7">
         <v>10</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2191,9 +2221,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2241,9 +2271,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2287,14 +2317,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A26" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.6328125" customWidth="1"/>
-    <col min="3" max="3" width="49.36328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.625" customWidth="1"/>
+    <col min="3" max="3" width="49.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2308,7 +2338,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -2319,7 +2349,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -2330,7 +2360,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -2341,7 +2371,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -2352,7 +2382,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -2363,7 +2393,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -2374,7 +2404,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -2385,7 +2415,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -2396,7 +2426,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>131</v>
       </c>
@@ -2407,7 +2437,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -2418,7 +2448,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -2429,7 +2459,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>134</v>
       </c>
@@ -2440,7 +2470,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>135</v>
       </c>
@@ -2451,7 +2481,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -2462,7 +2492,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -2473,7 +2503,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -2484,7 +2514,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -2495,7 +2525,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>140</v>
       </c>
@@ -2506,7 +2536,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>141</v>
       </c>
@@ -2517,7 +2547,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>142</v>
       </c>
@@ -2528,7 +2558,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>143</v>
       </c>
@@ -2539,7 +2569,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>144</v>
       </c>
@@ -2550,7 +2580,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>145</v>
       </c>
@@ -2561,7 +2591,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>146</v>
       </c>
@@ -2572,7 +2602,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>147</v>
       </c>
@@ -2583,7 +2613,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="94.5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>148</v>
       </c>
@@ -2594,7 +2624,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>149</v>
       </c>
@@ -2605,7 +2635,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>150</v>
       </c>
@@ -2616,7 +2646,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>151</v>
       </c>
@@ -2627,7 +2657,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>152</v>
       </c>
@@ -2638,7 +2668,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>153</v>
       </c>
@@ -2649,7 +2679,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>154</v>
       </c>
@@ -2660,7 +2690,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>155</v>
       </c>
@@ -2671,7 +2701,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>156</v>
       </c>
@@ -2682,7 +2712,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>157</v>
       </c>
@@ -2693,7 +2723,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>158</v>
       </c>
@@ -2704,7 +2734,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -2715,7 +2745,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>160</v>
       </c>
@@ -2726,7 +2756,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>161</v>
       </c>
@@ -2737,7 +2767,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>162</v>
       </c>
@@ -2748,7 +2778,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>163</v>
       </c>
@@ -2759,7 +2789,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>164</v>
       </c>

</xml_diff>